<commit_message>
Eingabe und erstes einstellen
</commit_message>
<xml_diff>
--- a/excel_datei_einstellungen/Leuchten.xlsx
+++ b/excel_datei_einstellungen/Leuchten.xlsx
@@ -30,19 +30,19 @@
     <t>#2</t>
   </si>
   <si>
-    <t>#3</t>
-  </si>
-  <si>
-    <t>#4</t>
-  </si>
-  <si>
     <t>Spannung [V]</t>
   </si>
   <si>
-    <t>Mininmalstrom [mA]</t>
-  </si>
-  <si>
-    <t>Maximalstrom [mA]</t>
+    <t>LED1 Mininmalstrom [mA]</t>
+  </si>
+  <si>
+    <t>LED1 Maximalstrom [mA]</t>
+  </si>
+  <si>
+    <t>LED2 Mininmalstrom [mA]</t>
+  </si>
+  <si>
+    <t>LED2 Maximalstrom [mA]</t>
   </si>
 </sst>
 </file>
@@ -66,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -122,16 +122,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -412,33 +422,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="24.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -451,8 +471,14 @@
       <c r="D2" s="1">
         <v>360</v>
       </c>
+      <c r="E2" s="5">
+        <v>1030</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1070</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -460,38 +486,16 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>1030</v>
+        <v>320</v>
       </c>
       <c r="D3" s="1">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
         <v>340</v>
       </c>
-      <c r="D4" s="1">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1030</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1070</v>
+      <c r="E3" s="5">
+        <v>1020</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>